<commit_message>
Recovered working state after stash confusion
</commit_message>
<xml_diff>
--- a/output/Table1.xlsx
+++ b/output/Table1.xlsx
@@ -444,19 +444,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>17718.55838682618</v>
+        <v>19792.54129835656</v>
       </c>
       <c r="C2">
-        <v>33872.19140473903</v>
+        <v>15066.47555447738</v>
       </c>
       <c r="D2">
-        <v>394.8438965349912</v>
+        <v>621.6720529563064</v>
       </c>
       <c r="E2">
-        <v>23883.16960588975</v>
+        <v>30290.74036012588</v>
       </c>
       <c r="F2">
-        <v>4809.974405273912</v>
+        <v>5701.982570874461</v>
       </c>
       <c r="G2">
         <v>92528.019626516</v>
@@ -467,19 +467,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>10903.85675608667</v>
+        <v>11692.00206736152</v>
       </c>
       <c r="C3">
-        <v>14714.37595330302</v>
+        <v>7093.838029203962</v>
       </c>
       <c r="D3">
-        <v>217.9206572447865</v>
+        <v>302.4603624540867</v>
       </c>
       <c r="E3">
-        <v>13748.14125008414</v>
+        <v>16324.85947714854</v>
       </c>
       <c r="F3">
-        <v>2811.242166023418</v>
+        <v>3109.280991178463</v>
       </c>
       <c r="G3">
         <v>86096</v>
@@ -490,19 +490,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>4927.854741818851</v>
+        <v>6131.186826176758</v>
       </c>
       <c r="C4">
-        <v>18332.75134893899</v>
+        <v>7385.415563697593</v>
       </c>
       <c r="D4">
-        <v>170.0256962936627</v>
+        <v>309.6276001236665</v>
       </c>
       <c r="E4">
-        <v>9781.831410898874</v>
+        <v>13515.18985424745</v>
       </c>
       <c r="F4">
-        <v>1786.813941233008</v>
+        <v>2312.637594047707</v>
       </c>
       <c r="G4">
         <v>3792.926263700311</v>
@@ -513,19 +513,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>863.6782889206661</v>
+        <v>946.1838048182954</v>
       </c>
       <c r="C5">
-        <v>782.88500249705</v>
+        <v>545.0428615758075</v>
       </c>
       <c r="D5">
-        <v>6.605042996541992</v>
+        <v>9.291590378553938</v>
       </c>
       <c r="E5">
-        <v>350.4507449067492</v>
+        <v>447.9448287298518</v>
       </c>
       <c r="F5">
-        <v>211.9182980174792</v>
+        <v>280.063985648286</v>
       </c>
       <c r="G5">
         <v>2639.093362815687</v>

</xml_diff>